<commit_message>
Remove CDATA from xlsx
</commit_message>
<xml_diff>
--- a/automation/vbz_frequenzen_hardbruecke/Frequenzen_Hardbruecke_Meta.xlsx
+++ b/automation/vbz_frequenzen_hardbruecke/Frequenzen_Hardbruecke_Meta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\OGD\Daten\Quelldaten\VBZ\vbz_frequenzen_hardbruecke\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\opendatazurich.github.io\automation\vbz_frequenzen_hardbruecke\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1013,152 +1013,45 @@
     <t>01.01.2020 - gestern</t>
   </si>
   <si>
-    <t>&lt;![CDATA[
-Zähldaten. Können laufend überschrieben werden.
-]]&gt;</t>
-  </si>
-  <si>
     <t>27.03.2020</t>
   </si>
   <si>
     <t>Situation:</t>
   </si>
   <si>
-    <t>&lt;![CDATA[
-Westkante:
-![Situationsplan Westkante](https://www.stadt-zuerich.ch/content/dam/stzh/portal/Deutsch/OGD/Bilder/ckan/zu-daten/vbz_Situation_Westkante.PNG)]
-Ostkante:
-![Situationsplan/Ostkante](https://www.stadt-zuerich.ch/content/dam/stzh/portal/Deutsch/OGD/Bilder/ckan/zu-daten/vbz_Situation_Ostkante.PNG)]
-]]&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;![CDATA[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="3" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Die Daten werden richtungsgetrennt ausgewiesen. 
+    <t>sachdaten, tabelle, öffentlicher verkehr, tram, bus, vbz, passagiere, pendler; fahrgastzahlen, öv, frequenzen, hardbücke</t>
+  </si>
+  <si>
+    <t>Bekannte Sensorausfälle:</t>
+  </si>
+  <si>
+    <t>Diese Daten beinhalten die Personenfrequenzen verschiedener Zähllinien an der VBZ-Haltestelle Hardbrücke, an der die Linie 33, 72, 83 und die Linie 8 verkehren.
+Mit diesem Test-System lassen sich Veränderungen an diesem speziellen Ort erkennen, welche aber nicht mit dem übrigen Netz oder dem Vorjahr verglichen werden können, um allfällige Effekte zu identifizieren.
+**Wichtiger Hinweis**: 
+Bitte beachten Sie die Hinweise unter **«Bekannte Sensorausfälle»** ob bei einer Datenanalyse im Untersuchungszeitraum ein Sensorausfall stattgefunden hat.</t>
+  </si>
+  <si>
+    <t>Zähldaten. Können laufend überschrieben werden.</t>
+  </si>
+  <si>
+    <t>Die Daten werden richtungsgetrennt ausgewiesen. 
 - "Ost" bezeichnet die Haltestelle Hardbrücke mit Fahrtrichtung Schiffbau.
 - "West" bezeichnet die Haltestelle Hardbrücke mit Fahrtrichtung Hardplatz. 
 Zudem werden die Frequenzen an vier verschiedenen Zähllinien erfasst. 
 - "Süd" bezeichnet die Zähllinie im Süden der Haltestelle. Es werden alle Personen erfasst, die vom Hardplatz kommend die VBZ-Haltestelle betreten bzw. die Haltestelle in diese Richtung verlassen.
 - "Nord" bezeichnet die Zähllinie im Norden der Haltestelle. Es werden alle Persoenen erfasst, die via Fussgängerrampe im Norden die VBZ-Haltestelle betreten/verlassen.
 - "SBB", bezeichnet die Zähllinie mit Zugang zur S-Bahnstation Hardbrücke. Es werden alle Personen erfasst, die von der SBB kommend die VBZ-Haltestelle betreten bzw. die Haltestelle in diese Richtung verlassen.
-- "VBZ", bezeichnet die Zähllinie mit den VBZ-Frequenzen. Es werden alle Persoenen erfasst, die von einem VBZ-Fahrzeug die VBZ-Haltestelle betreten bzw. die Haltestelle durch Einstieg in ein VBZ-Fahrzeug verlassen.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]]&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>sachdaten, tabelle, öffentlicher verkehr, tram, bus, vbz, passagiere, pendler; fahrgastzahlen, öv, frequenzen, hardbücke</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;![CDATA[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="3" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="3" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Diese Daten beinhalten die Personenfrequenzen verschiedener Zähllinien an der VBZ-Haltestelle Hardbrücke, an der die Linie 33, 72, 83 und die Linie 8 verkehren.
-Mit diesem Test-System lassen sich Veränderungen an diesem speziellen Ort erkennen, welche aber nicht mit dem übrigen Netz oder dem Vorjahr verglichen werden können, um allfällige Effekte zu identifizieren.
-**Wichtiger Hinweis**: 
-Bitte beachten Sie die Hinweise unter **«Bekannte Sensorausfälle»** ob bei einer Datenanalyse im Untersuchungszeitraum ein Sensorausfall stattgefunden hat.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]]&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;![CDATA[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="3" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- 01.08. - 13.08.2020: Sensorausfall an der Hardbrücke (Ost-Seite) ausgefallen. Dies hat zur Folge, dass die Daten für die SBB-Zähllinie Ost (Attribut `Ost-SBB total`) in diesem Zeitraum fehlen.
-**Genereller Hinweis:** Das Zählsystem an der Hardbrücke ist erst seit Q4 2019 im Betrieb. Es kann generell zu einzelnen Datenlücken kommen. Die VBZ arbeitet laufend daran, bekannte Datenlücken wenn möglich zu minimieren. Die Daten können somit stets überschrieben werden.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]]&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>Bekannte Sensorausfälle:</t>
+- "VBZ", bezeichnet die Zähllinie mit den VBZ-Frequenzen. Es werden alle Persoenen erfasst, die von einem VBZ-Fahrzeug die VBZ-Haltestelle betreten bzw. die Haltestelle durch Einstieg in ein VBZ-Fahrzeug verlassen.</t>
+  </si>
+  <si>
+    <t>- 01.08. - 13.08.2020: Sensorausfall an der Hardbrücke (Ost-Seite) ausgefallen. Dies hat zur Folge, dass die Daten für die SBB-Zähllinie Ost (Attribut `Ost-SBB total`) in diesem Zeitraum fehlen.
+**Genereller Hinweis:** Das Zählsystem an der Hardbrücke ist erst seit Q4 2019 im Betrieb. Es kann generell zu einzelnen Datenlücken kommen. Die VBZ arbeitet laufend daran, bekannte Datenlücken wenn möglich zu minimieren. Die Daten können somit stets überschrieben werden.</t>
+  </si>
+  <si>
+    <t>Westkante:
+![Situationsplan Westkante](https://www.stadt-zuerich.ch/content/dam/stzh/portal/Deutsch/OGD/Bilder/ckan/zu-daten/vbz_Situation_Westkante.PNG)]
+Ostkante:
+![Situationsplan/Ostkante](https://www.stadt-zuerich.ch/content/dam/stzh/portal/Deutsch/OGD/Bilder/ckan/zu-daten/vbz_Situation_Ostkante.PNG)]</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1434,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
@@ -1654,6 +1547,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1970,7 +1866,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2026,7 +1922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>54</v>
       </c>
@@ -2036,8 +1932,8 @@
       <c r="C3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>192</v>
+      <c r="D3" s="34" t="s">
+        <v>190</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
@@ -2150,7 +2046,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>34</v>
       </c>
@@ -2161,7 +2057,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
@@ -2179,7 +2075,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="7" t="s">
@@ -2249,7 +2145,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
@@ -2322,7 +2218,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="255" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="229.5" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>51</v>
       </c>
@@ -2330,7 +2226,7 @@
         <v>172</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="7"/>
@@ -2338,14 +2234,14 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="C22" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="40" t="s">
         <v>193</v>
       </c>
       <c r="D22" s="1"/>
@@ -2354,15 +2250,15 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="153" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="7"/>
@@ -3178,21 +3074,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008CBAF0EEED2F5B4AB4463B97C2AD2B71" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="d2bc9691d179cb44d4ba77bdf8fcfb4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c4a6dd5ef775a5269b08f7de37f93f">
     <xsd:element name="properties">
@@ -3306,10 +3187,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3330,17 +3234,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Störungsmeldung für Hardbrücke für die Zähllinien WEST
</commit_message>
<xml_diff>
--- a/automation/vbz_frequenzen_hardbruecke/Frequenzen_Hardbruecke_Meta.xlsx
+++ b/automation/vbz_frequenzen_hardbruecke/Frequenzen_Hardbruecke_Meta.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\opendatazurich.github.io\automation\vbz_frequenzen_hardbruecke\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\sszsim\opendatazurich\opendatazurich.github.io\automation\vbz_frequenzen_hardbruecke\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5B89B9-B716-4787-8B98-D02D27197D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-45" windowWidth="21225" windowHeight="12540"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="14" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="215">
   <si>
     <t>Erstmalige Veröffentlichung</t>
   </si>
@@ -1107,11 +1108,17 @@
 Ostkante:
 ![Situationsplan/Ostkante](https://www.stadt-zuerich.ch/content/dam/stzh/portal/Deutsch/OGD/Bilder/ckan/zu-daten/vbz_Situation_Ostkante.PNG)</t>
   </si>
+  <si>
+    <t>Störungen:</t>
+  </si>
+  <si>
+    <t>- Zählwerte ab 1.1.2023 auf dem **Perron "West"** sind **nicht korrekt**. Bitte verwenden Sie die absoluten Werte derzeit nicht, bis das Problem behoben ist.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1494,7 +1501,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
@@ -1615,16 +1622,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
-    <cellStyle name="Standard 3" xfId="2"/>
-    <cellStyle name="Standard 4" xfId="3"/>
-    <cellStyle name="Standard 5" xfId="4"/>
-    <cellStyle name="Standard 6" xfId="5"/>
-    <cellStyle name="Standard 7" xfId="7"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Standard 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Standard 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Standard 5" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Standard 6" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Standard 7" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1645,18 +1655,24 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2600325</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Grafik 2" descr="cid:image002.png@01D60363.7EDEE1F0"/>
+        <xdr:cNvPr id="2" name="Grafik 2" descr="cid:image002.png@01D60363.7EDEE1F0">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1925,26 +1941,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="14.09765625" style="11" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="66.875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="53.625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="8.75" style="5" customWidth="1"/>
-    <col min="6" max="6" width="88.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="50.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.8984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="53.59765625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="8.69921875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="88.8984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="50.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="255.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
@@ -1967,7 +1983,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
@@ -1985,7 +2001,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>54</v>
       </c>
@@ -2003,7 +2019,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
@@ -2021,7 +2037,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
@@ -2037,7 +2053,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
@@ -2055,7 +2071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>31</v>
       </c>
@@ -2073,7 +2089,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
@@ -2091,7 +2107,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>33</v>
       </c>
@@ -2109,7 +2125,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>34</v>
       </c>
@@ -2127,7 +2143,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>35</v>
       </c>
@@ -2145,7 +2161,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
@@ -2161,7 +2177,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>38</v>
       </c>
@@ -2179,7 +2195,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>39</v>
       </c>
@@ -2197,7 +2213,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="4" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>49</v>
       </c>
@@ -2215,7 +2231,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>52</v>
       </c>
@@ -2233,7 +2249,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>129</v>
       </c>
@@ -2251,14 +2267,14 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>37</v>
       </c>
@@ -2271,7 +2287,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>11</v>
       </c>
@@ -2281,7 +2297,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="229.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>51</v>
       </c>
@@ -2297,248 +2313,262 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="82.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>189</v>
+        <v>213</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>214</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="38" t="s">
-        <v>184</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>212</v>
+      <c r="B23" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>189</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
+      <c r="F23" s="22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="118.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>212</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9" t="s">
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-      <c r="B27" s="13" t="s">
+    <row r="28" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="B28" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C28" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D28" s="13" t="s">
         <v>28</v>
-      </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>177</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="1:6" s="4" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+      <c r="F30" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" s="4" customFormat="1" ht="171.6" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C32" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D32" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="11"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="7"/>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
-      <c r="B35" s="3" t="s">
-        <v>164</v>
-      </c>
+      <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
-      <c r="B36" s="3"/>
+      <c r="B36" s="3" t="s">
+        <v>164</v>
+      </c>
       <c r="C36" s="3"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B38" s="13" t="s">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B39" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C39" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="8" t="s">
+      <c r="D39" s="13"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="8" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>158</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>162</v>
+      </c>
       <c r="D41" s="12"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F45"/>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F46"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.98425196850393704" bottom="0.59055118110236227" header="0.39370078740157483" footer="0.27559055118110237"/>
@@ -2548,33 +2578,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.375" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.875" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.375" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.375" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.625" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.375" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.75" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.625" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.875" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.3984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.8984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.3984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.09765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.3984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.8984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.3984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.69921875" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.8984375" style="23" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>70</v>
       </c>
@@ -2582,7 +2612,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>133</v>
       </c>
@@ -2590,7 +2620,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>134</v>
       </c>
@@ -2598,7 +2628,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>135</v>
       </c>
@@ -2606,7 +2636,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>136</v>
       </c>
@@ -2614,7 +2644,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>137</v>
       </c>
@@ -2622,7 +2652,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>138</v>
       </c>
@@ -2630,7 +2660,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>139</v>
       </c>
@@ -2638,7 +2668,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>140</v>
       </c>
@@ -2646,7 +2676,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>141</v>
       </c>
@@ -2654,7 +2684,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>142</v>
       </c>
@@ -2662,7 +2692,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>143</v>
       </c>
@@ -2670,7 +2700,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>144</v>
       </c>
@@ -2678,7 +2708,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>145</v>
       </c>
@@ -2686,7 +2716,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>146</v>
       </c>
@@ -2694,7 +2724,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>147</v>
       </c>
@@ -2702,7 +2732,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>148</v>
       </c>
@@ -2710,7 +2740,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>149</v>
       </c>
@@ -2718,7 +2748,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>150</v>
       </c>
@@ -2726,7 +2756,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>151</v>
       </c>
@@ -2734,19 +2764,19 @@
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>128</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A24" r:id="rId1" location="metadata"/>
+    <hyperlink ref="A24" r:id="rId1" location="metadata" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.27559055118110237"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2754,21 +2784,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5" style="23" customWidth="1"/>
-    <col min="2" max="2" width="5.625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="5.59765625" style="23" customWidth="1"/>
     <col min="3" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>70</v>
       </c>
@@ -2776,27 +2806,27 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>71</v>
       </c>
@@ -2804,19 +2834,19 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>128</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A11" r:id="rId1" location="metadata"/>
+    <hyperlink ref="A11" r:id="rId1" location="metadata" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.27559055118110237"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2824,21 +2854,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.375" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.25" style="23" customWidth="1"/>
+    <col min="1" max="1" width="35.3984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.19921875" style="23" customWidth="1"/>
     <col min="3" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>70</v>
       </c>
@@ -2846,123 +2876,123 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
     </row>
-    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
     </row>
-    <row r="23" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
     </row>
-    <row r="24" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
     </row>
-    <row r="25" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
     </row>
-    <row r="26" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
     </row>
-    <row r="27" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1" location="metadata"/>
+    <hyperlink ref="A21" r:id="rId1" location="metadata" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.27559055118110237"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2970,22 +3000,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5" style="23" customWidth="1"/>
-    <col min="2" max="2" width="5.375" style="23" customWidth="1"/>
-    <col min="3" max="3" width="58.625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.3984375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="58.59765625" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>70</v>
       </c>
@@ -2996,7 +3026,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>87</v>
       </c>
@@ -3008,7 +3038,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>88</v>
       </c>
@@ -3020,7 +3050,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>89</v>
       </c>
@@ -3032,7 +3062,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>90</v>
       </c>
@@ -3044,7 +3074,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>91</v>
       </c>
@@ -3056,7 +3086,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>92</v>
       </c>
@@ -3068,7 +3098,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>93</v>
       </c>
@@ -3080,7 +3110,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>94</v>
       </c>
@@ -3092,7 +3122,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>95</v>
       </c>
@@ -3104,7 +3134,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>96</v>
       </c>
@@ -3116,7 +3146,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>97</v>
       </c>
@@ -3128,7 +3158,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>98</v>
       </c>
@@ -3140,7 +3170,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>99</v>
       </c>
@@ -3152,7 +3182,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>100</v>
       </c>
@@ -3164,7 +3194,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>101</v>
       </c>
@@ -3176,12 +3206,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>128</v>
       </c>
@@ -3189,7 +3219,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A22" r:id="rId1" location="metadata"/>
+    <hyperlink ref="A22" r:id="rId1" location="metadata" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.27559055118110237"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Update der Metadaten der VBZ-Fahrgastfrequenzen an der Hardbrücke, da die Sensoren seit 20.12.2023 nicht mehr laufen.
</commit_message>
<xml_diff>
--- a/automation/vbz_frequenzen_hardbruecke/Frequenzen_Hardbruecke_Meta.xlsx
+++ b/automation/vbz_frequenzen_hardbruecke/Frequenzen_Hardbruecke_Meta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\sszsim\opendatazurich\opendatazurich.github.io\automation\vbz_frequenzen_hardbruecke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5B89B9-B716-4787-8B98-D02D27197D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC81F55A-B58F-4139-82EB-690DA5ABD059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="14" r:id="rId1"/>
@@ -999,10 +999,6 @@
 - "VBZ", bezeichnet die Zähllinie mit den VBZ-Frequenzen. Es werden alle Persoenen erfasst, die von einem VBZ-Fahrzeug die VBZ-Haltestelle betreten bzw. die Haltestelle durch Einstieg in ein VBZ-Fahrzeug verlassen.</t>
   </si>
   <si>
-    <t>- 01.08. - 13.08.2020: Sensorausfall an der Hardbrücke (Ost-Seite) ausgefallen. Dies hat zur Folge, dass die Daten für die SBB-Zähllinie Ost (Attribut `Ost-SBB total`) in diesem Zeitraum fehlen.
-**Genereller Hinweis:** Das Zählsystem an der Hardbrücke ist erst seit Q4 2019 im Betrieb. Es kann generell zu einzelnen Datenlücken kommen. Die VBZ arbeitet laufend daran, bekannte Datenlücken wenn möglich zu minimieren. Die Daten können somit stets überschrieben werden.</t>
-  </si>
-  <si>
     <t>sachdaten, tabelle, öffentlicher verkehr, tram, bus, vbz, passagiere, pendler, fahrgastzahlen, öv, frequenzen, hardbücke</t>
   </si>
   <si>
@@ -1113,6 +1109,11 @@
   </si>
   <si>
     <t>- Zählwerte ab 1.1.2023 auf dem **Perron "West"** sind **nicht korrekt**. Bitte verwenden Sie die absoluten Werte derzeit nicht, bis das Problem behoben ist.</t>
+  </si>
+  <si>
+    <t>- **20.12.2023 - ca. 15.01.2024**: Wegen Unterhaltsarbeiten lieferte die Schnittstelle keine Zähldaten.
+- 01.08. - 13.08.2020: Sensorausfall an der Hardbrücke (Ost-Seite) ausgefallen. Dies hat zur Folge, dass die Daten für die SBB-Zähllinie Ost (Attribut `Ost-SBB total`) in diesem Zeitraum fehlen.
+**Genereller Hinweis:** Das Zählsystem an der Hardbrücke ist erst seit Q4 2019 im Betrieb. Es kann generell zu einzelnen Datenlücken kommen. Die VBZ arbeitet laufend daran, bekannte Datenlücken wenn möglich zu minimieren. Die Daten können somit stets überschrieben werden.</t>
   </si>
 </sst>
 </file>
@@ -1945,22 +1946,22 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.09765625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="14.08203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="66.8984375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="53.59765625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="8.69921875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="88.8984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="50.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.9140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="53.58203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="88.9140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="50.4140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="255.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
@@ -2001,7 +2002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="171.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="169" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>54</v>
       </c>
@@ -2019,7 +2020,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
@@ -2030,14 +2031,14 @@
         <v>14</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
@@ -2053,7 +2054,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
@@ -2071,7 +2072,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>31</v>
       </c>
@@ -2089,7 +2090,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
@@ -2107,7 +2108,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>33</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>34</v>
       </c>
@@ -2143,7 +2144,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>35</v>
       </c>
@@ -2161,7 +2162,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
@@ -2177,7 +2178,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>38</v>
       </c>
@@ -2195,7 +2196,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>39</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>49</v>
       </c>
@@ -2224,14 +2225,14 @@
         <v>14</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>52</v>
       </c>
@@ -2249,7 +2250,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
         <v>129</v>
       </c>
@@ -2267,14 +2268,14 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>37</v>
       </c>
@@ -2287,7 +2288,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
         <v>11</v>
       </c>
@@ -2297,7 +2298,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="237.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="225" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>51</v>
       </c>
@@ -2313,21 +2314,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="82.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="82.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" s="42" t="s">
         <v>213</v>
-      </c>
-      <c r="C22" s="42" t="s">
-        <v>214</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="7"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="137.5" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>51</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>185</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="7"/>
@@ -2343,7 +2344,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>51</v>
       </c>
@@ -2351,18 +2352,18 @@
         <v>184</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="1"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2370,7 +2371,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>29</v>
       </c>
@@ -2386,7 +2387,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="13" t="s">
         <v>26</v>
@@ -2402,7 +2403,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>30</v>
       </c>
@@ -2420,7 +2421,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
@@ -2438,7 +2439,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" s="4" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>30</v>
       </c>
@@ -2453,7 +2454,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:6" s="4" customFormat="1" ht="171.6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="4" customFormat="1" ht="162.5" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
@@ -2468,28 +2469,28 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A34" s="11"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A35" s="11"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
       <c r="B36" s="3" t="s">
         <v>164</v>
@@ -2498,14 +2499,14 @@
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>155</v>
       </c>
@@ -2519,7 +2520,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="25" x14ac:dyDescent="0.3">
       <c r="B39" s="13" t="s">
         <v>156</v>
       </c>
@@ -2532,7 +2533,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>158</v>
       </c>
@@ -2546,7 +2547,7 @@
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>158</v>
       </c>
@@ -2560,14 +2561,14 @@
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F46"/>
     </row>
   </sheetData>
@@ -2585,191 +2586,191 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.3984375" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.59765625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.8984375" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.59765625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.3984375" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.09765625" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.3984375" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.8984375" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.59765625" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.3984375" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.69921875" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.59765625" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.8984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.4140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.58203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.58203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.9140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.58203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.4140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.08203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.4140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.9140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.58203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.4140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.58203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.9140625" style="23" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>70</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>133</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>134</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>135</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>136</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>137</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>138</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>139</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>140</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>141</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>142</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>143</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>144</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>145</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>146</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>147</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>148</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>149</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
         <v>150</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
         <v>151</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="32" t="s">
         <v>128</v>
       </c>
@@ -2791,14 +2792,14 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5" style="23" customWidth="1"/>
-    <col min="2" max="2" width="5.59765625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="5.58203125" style="23" customWidth="1"/>
     <col min="3" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>70</v>
       </c>
@@ -2806,27 +2807,27 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>71</v>
       </c>
@@ -2834,12 +2835,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>128</v>
       </c>
@@ -2861,14 +2862,14 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.3984375" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.19921875" style="23" customWidth="1"/>
+    <col min="1" max="1" width="35.4140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" style="23" customWidth="1"/>
     <col min="3" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>70</v>
       </c>
@@ -2876,118 +2877,118 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A18" s="25"/>
     </row>
-    <row r="19" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="32" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A22" s="25"/>
     </row>
-    <row r="23" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A23" s="25"/>
     </row>
-    <row r="24" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A24" s="25"/>
     </row>
-    <row r="25" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A25" s="25"/>
     </row>
-    <row r="26" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A26" s="25"/>
     </row>
-    <row r="27" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A27" s="25"/>
     </row>
   </sheetData>
@@ -3007,15 +3008,15 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.5" style="23" customWidth="1"/>
-    <col min="2" max="2" width="5.3984375" style="23" customWidth="1"/>
-    <col min="3" max="3" width="58.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.4140625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="58.58203125" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>70</v>
       </c>
@@ -3026,7 +3027,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>87</v>
       </c>
@@ -3038,7 +3039,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>88</v>
       </c>
@@ -3050,7 +3051,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>89</v>
       </c>
@@ -3062,7 +3063,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>90</v>
       </c>
@@ -3074,7 +3075,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>91</v>
       </c>
@@ -3086,7 +3087,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>92</v>
       </c>
@@ -3098,7 +3099,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>93</v>
       </c>
@@ -3110,7 +3111,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>94</v>
       </c>
@@ -3122,7 +3123,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>95</v>
       </c>
@@ -3134,7 +3135,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>96</v>
       </c>
@@ -3146,7 +3147,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>97</v>
       </c>
@@ -3158,7 +3159,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>98</v>
       </c>
@@ -3170,7 +3171,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>99</v>
       </c>
@@ -3182,7 +3183,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>100</v>
       </c>
@@ -3194,7 +3195,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>101</v>
       </c>
@@ -3206,12 +3207,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="s">
         <v>128</v>
       </c>
@@ -3227,6 +3228,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008CBAF0EEED2F5B4AB4463B97C2AD2B71" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="d2bc9691d179cb44d4ba77bdf8fcfb4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c4a6dd5ef775a5269b08f7de37f93f">
     <xsd:element name="properties">
@@ -3340,12 +3347,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3356,6 +3357,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3371,21 +3387,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fitting URL of the Hardbrücke Picture Links
</commit_message>
<xml_diff>
--- a/automation/vbz_frequenzen_hardbruecke/Frequenzen_Hardbruecke_Meta.xlsx
+++ b/automation/vbz_frequenzen_hardbruecke/Frequenzen_Hardbruecke_Meta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\sszsim\opendatazurich\opendatazurich.github.io\automation\vbz_frequenzen_hardbruecke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC81F55A-B58F-4139-82EB-690DA5ABD059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B91F59-0042-4967-99A1-BE107B1A56E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31236" yWindow="1368" windowWidth="25380" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="14" r:id="rId1"/>
@@ -1099,12 +1099,6 @@
     <t>arbeit-und-erwerb</t>
   </si>
   <si>
-    <t>Westkante:
-![Situationsplan Westkante](https://www.stadt-zuerich.ch/content/dam/stzh/portal/Deutsch/OGD/Bilder/ckan/zu-daten/vbz_Situation_Westkante.PNG)
-Ostkante:
-![Situationsplan/Ostkante](https://www.stadt-zuerich.ch/content/dam/stzh/portal/Deutsch/OGD/Bilder/ckan/zu-daten/vbz_Situation_Ostkante.PNG)</t>
-  </si>
-  <si>
     <t>Störungen:</t>
   </si>
   <si>
@@ -1114,6 +1108,12 @@
     <t>- **20.12.2023 - ca. 15.01.2024**: Wegen Unterhaltsarbeiten lieferte die Schnittstelle keine Zähldaten.
 - 01.08. - 13.08.2020: Sensorausfall an der Hardbrücke (Ost-Seite) ausgefallen. Dies hat zur Folge, dass die Daten für die SBB-Zähllinie Ost (Attribut `Ost-SBB total`) in diesem Zeitraum fehlen.
 **Genereller Hinweis:** Das Zählsystem an der Hardbrücke ist erst seit Q4 2019 im Betrieb. Es kann generell zu einzelnen Datenlücken kommen. Die VBZ arbeitet laufend daran, bekannte Datenlücken wenn möglich zu minimieren. Die Daten können somit stets überschrieben werden.</t>
+  </si>
+  <si>
+    <t>Westkante:
+![Situationsplan Westkante](https://www.stadt-zuerich.ch/content/dam/web/de/politik-verwaltung/statistik-und-daten/open-government-data/bilder/datenkatalog/vbz/vbz_Situation_Westkante.PNG)
+Ostkante:
+![Situationsplan/Ostkante](https://www.stadt-zuerich.ch/content/dam/web/de/politik-verwaltung/statistik-und-daten/open-government-data/bilder/datenkatalog/vbz/vbz_Situation_Ostkante.PNG)</t>
   </si>
 </sst>
 </file>
@@ -1502,7 +1502,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
@@ -1625,6 +1625,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1945,8 +1948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2319,10 +2322,10 @@
         <v>51</v>
       </c>
       <c r="B22" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="C22" s="42" t="s">
         <v>212</v>
-      </c>
-      <c r="C22" s="42" t="s">
-        <v>213</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="7"/>
@@ -2336,7 +2339,7 @@
         <v>185</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="7"/>
@@ -2352,9 +2355,9 @@
         <v>184</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>211</v>
-      </c>
-      <c r="D24" s="1"/>
+        <v>214</v>
+      </c>
+      <c r="D24" s="43"/>
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3228,12 +3231,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008CBAF0EEED2F5B4AB4463B97C2AD2B71" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="d2bc9691d179cb44d4ba77bdf8fcfb4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c4a6dd5ef775a5269b08f7de37f93f">
     <xsd:element name="properties">
@@ -3347,6 +3344,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3357,21 +3360,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3387,6 +3375,21 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update Störungen in metadata
</commit_message>
<xml_diff>
--- a/automation/vbz_frequenzen_hardbruecke/Frequenzen_Hardbruecke_Meta.xlsx
+++ b/automation/vbz_frequenzen_hardbruecke/Frequenzen_Hardbruecke_Meta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\sszsim\opendatazurich\opendatazurich.github.io\automation\vbz_frequenzen_hardbruecke\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszgua\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B91F59-0042-4967-99A1-BE107B1A56E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB8B9F5-1B80-4C9C-9BF6-7994F0B77107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31236" yWindow="1368" windowWidth="25380" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="-120" windowWidth="27855" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="14" r:id="rId1"/>
@@ -919,9 +919,6 @@
     <t>Verkehrsbetriebe Zürich, Departement der Industriellen Betriebe</t>
   </si>
   <si>
-    <t xml:space="preserve">Information zum Datensatz </t>
-  </si>
-  <si>
     <t>In</t>
   </si>
   <si>
@@ -1102,18 +1099,22 @@
     <t>Störungen:</t>
   </si>
   <si>
-    <t>- Zählwerte ab 1.1.2023 auf dem **Perron "West"** sind **nicht korrekt**. Bitte verwenden Sie die absoluten Werte derzeit nicht, bis das Problem behoben ist.</t>
-  </si>
-  <si>
-    <t>- **20.12.2023 - ca. 15.01.2024**: Wegen Unterhaltsarbeiten lieferte die Schnittstelle keine Zähldaten.
-- 01.08. - 13.08.2020: Sensorausfall an der Hardbrücke (Ost-Seite) ausgefallen. Dies hat zur Folge, dass die Daten für die SBB-Zähllinie Ost (Attribut `Ost-SBB total`) in diesem Zeitraum fehlen.
-**Genereller Hinweis:** Das Zählsystem an der Hardbrücke ist erst seit Q4 2019 im Betrieb. Es kann generell zu einzelnen Datenlücken kommen. Die VBZ arbeitet laufend daran, bekannte Datenlücken wenn möglich zu minimieren. Die Daten können somit stets überschrieben werden.</t>
-  </si>
-  <si>
     <t>Westkante:
 ![Situationsplan Westkante](https://www.stadt-zuerich.ch/content/dam/web/de/politik-verwaltung/statistik-und-daten/open-government-data/bilder/datenkatalog/vbz/vbz_Situation_Westkante.PNG)
 Ostkante:
 ![Situationsplan/Ostkante](https://www.stadt-zuerich.ch/content/dam/web/de/politik-verwaltung/statistik-und-daten/open-government-data/bilder/datenkatalog/vbz/vbz_Situation_Ostkante.PNG)</t>
+  </si>
+  <si>
+    <t>- Die absoluten Zählwerte auf dem Perron **Ost** sind von Januar 2023 bis und mit Juli 2023 fehlerbehaftet
+- Die absoluten Zählwerte auf dem Perron **West** sind von Dezember 2019 bis und mit Dezember 2023 fehlerbehaftet</t>
+  </si>
+  <si>
+    <t>- **20.12.2023 - ca. 15.01.2024**: Wegen Unterhaltsarbeiten lieferte die Schnittstelle keine Zähldaten.
+- **01.08. - 13.08.2020**: Sensorausfall an der Hardbrücke (Ost-Seite) ausgefallen. Dies hat zur Folge, dass die Daten für die SBB-Zähllinie Ost (Attribut `Ost-SBB total`) in diesem Zeitraum fehlen.
+**Genereller Hinweis:** Das Zählsystem an der Hardbrücke ist erst seit Q4 2019 im Betrieb. Es kann generell zu einzelnen Datenlücken kommen. Die VBZ arbeitet laufend daran, bekannte Datenlücken wenn möglich zu minimieren. Die Daten können somit stets überschrieben werden.</t>
+  </si>
+  <si>
+    <t>Information zum Datensatz</t>
   </si>
 </sst>
 </file>
@@ -1948,23 +1949,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.08203125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="14.125" style="11" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="66.9140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="53.58203125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="88.9140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="50.4140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="53.625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="88.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="50.375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="255.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
@@ -1987,7 +1988,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
@@ -1998,14 +1999,14 @@
         <v>14</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="169" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>54</v>
       </c>
@@ -2016,14 +2017,14 @@
         <v>14</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
@@ -2034,14 +2035,14 @@
         <v>14</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
@@ -2057,7 +2058,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
@@ -2075,7 +2076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>31</v>
       </c>
@@ -2093,7 +2094,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>33</v>
       </c>
@@ -2122,14 +2123,14 @@
         <v>14</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>34</v>
       </c>
@@ -2140,14 +2141,14 @@
         <v>15</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>35</v>
       </c>
@@ -2158,14 +2159,14 @@
         <v>15</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
@@ -2181,7 +2182,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>38</v>
       </c>
@@ -2199,7 +2200,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>39</v>
       </c>
@@ -2217,7 +2218,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>49</v>
       </c>
@@ -2228,14 +2229,14 @@
         <v>14</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>52</v>
       </c>
@@ -2253,7 +2254,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
         <v>129</v>
       </c>
@@ -2271,14 +2272,14 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>37</v>
       </c>
@@ -2291,7 +2292,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" s="13" t="s">
         <v>11</v>
       </c>
@@ -2301,15 +2302,15 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="225" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="229.5" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>169</v>
+        <v>214</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="7"/>
@@ -2317,12 +2318,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="82.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="82.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C22" s="42" t="s">
         <v>212</v>
@@ -2331,12 +2332,12 @@
       <c r="E22" s="7"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" ht="137.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C23" s="40" t="s">
         <v>213</v>
@@ -2347,26 +2348,26 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="112.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D24" s="43"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="1"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2374,7 +2375,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>29</v>
       </c>
@@ -2390,7 +2391,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="13" t="s">
         <v>26</v>
@@ -2406,94 +2407,94 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="4" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:6" s="4" customFormat="1" ht="162.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="4" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
       <c r="B36" s="3" t="s">
         <v>164</v>
@@ -2502,14 +2503,14 @@
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>155</v>
       </c>
@@ -2523,7 +2524,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" ht="25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B39" s="13" t="s">
         <v>156</v>
       </c>
@@ -2536,7 +2537,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>158</v>
       </c>
@@ -2550,7 +2551,7 @@
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>158</v>
       </c>
@@ -2564,14 +2565,14 @@
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F46"/>
     </row>
   </sheetData>
@@ -2589,191 +2590,191 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.4140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.58203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.58203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.9140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.58203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.4140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.08203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.4140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.9140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.58203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.4140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.58203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.9140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.375" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.375" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.875" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.375" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.625" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.625" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.875" style="23" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>70</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>133</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
         <v>134</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>135</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>136</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>137</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>138</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>139</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
         <v>140</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
         <v>141</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
         <v>142</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
         <v>143</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
         <v>144</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
         <v>145</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
         <v>146</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
         <v>147</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="29" t="s">
         <v>148</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="s">
         <v>149</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="29" t="s">
         <v>150</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="29" t="s">
         <v>151</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>128</v>
       </c>
@@ -2795,14 +2796,14 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" style="23" customWidth="1"/>
-    <col min="2" max="2" width="5.58203125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="5.625" style="23" customWidth="1"/>
     <col min="3" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>70</v>
       </c>
@@ -2810,27 +2811,27 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
         <v>71</v>
       </c>
@@ -2838,12 +2839,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>128</v>
       </c>
@@ -2865,14 +2866,14 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.4140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" style="23" customWidth="1"/>
+    <col min="1" max="1" width="35.375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.125" style="23" customWidth="1"/>
     <col min="3" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>70</v>
       </c>
@@ -2880,118 +2881,118 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="25"/>
     </row>
-    <row r="19" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="25"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="25"/>
     </row>
-    <row r="23" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="25"/>
     </row>
-    <row r="24" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="25"/>
     </row>
-    <row r="25" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="25"/>
     </row>
-    <row r="26" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="25"/>
     </row>
-    <row r="27" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="25"/>
     </row>
   </sheetData>
@@ -3011,15 +3012,15 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" style="23" customWidth="1"/>
-    <col min="2" max="2" width="5.4140625" style="23" customWidth="1"/>
-    <col min="3" max="3" width="58.58203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="58.625" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>70</v>
       </c>
@@ -3030,7 +3031,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>87</v>
       </c>
@@ -3042,7 +3043,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
         <v>88</v>
       </c>
@@ -3054,7 +3055,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>89</v>
       </c>
@@ -3066,7 +3067,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>90</v>
       </c>
@@ -3078,7 +3079,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>91</v>
       </c>
@@ -3090,7 +3091,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
         <v>92</v>
       </c>
@@ -3102,7 +3103,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>93</v>
       </c>
@@ -3114,7 +3115,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
         <v>94</v>
       </c>
@@ -3126,7 +3127,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
         <v>95</v>
       </c>
@@ -3138,7 +3139,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
         <v>96</v>
       </c>
@@ -3150,7 +3151,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
         <v>97</v>
       </c>
@@ -3162,7 +3163,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
         <v>98</v>
       </c>
@@ -3174,7 +3175,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
         <v>99</v>
       </c>
@@ -3186,7 +3187,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
         <v>100</v>
       </c>
@@ -3198,7 +3199,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
         <v>101</v>
       </c>
@@ -3210,12 +3211,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
Anpassung URL bei VBZ Hardbrücke
</commit_message>
<xml_diff>
--- a/automation/vbz_frequenzen_hardbruecke/Frequenzen_Hardbruecke_Meta.xlsx
+++ b/automation/vbz_frequenzen_hardbruecke/Frequenzen_Hardbruecke_Meta.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszgua\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\sszsim\1_github_odz\opendatazurich.github.io\automation\vbz_frequenzen_hardbruecke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB8B9F5-1B80-4C9C-9BF6-7994F0B77107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D3BE67-B8BF-4104-9826-3EB1B41EFF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="-120" windowWidth="27855" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="14" r:id="rId1"/>
@@ -1099,12 +1099,6 @@
     <t>Störungen:</t>
   </si>
   <si>
-    <t>Westkante:
-![Situationsplan Westkante](https://www.stadt-zuerich.ch/content/dam/web/de/politik-verwaltung/statistik-und-daten/open-government-data/bilder/datenkatalog/vbz/vbz_Situation_Westkante.PNG)
-Ostkante:
-![Situationsplan/Ostkante](https://www.stadt-zuerich.ch/content/dam/web/de/politik-verwaltung/statistik-und-daten/open-government-data/bilder/datenkatalog/vbz/vbz_Situation_Ostkante.PNG)</t>
-  </si>
-  <si>
     <t>- Die absoluten Zählwerte auf dem Perron **Ost** sind von Januar 2023 bis und mit Juli 2023 fehlerbehaftet
 - Die absoluten Zählwerte auf dem Perron **West** sind von Dezember 2019 bis und mit Dezember 2023 fehlerbehaftet</t>
   </si>
@@ -1115,6 +1109,12 @@
   </si>
   <si>
     <t>Information zum Datensatz</t>
+  </si>
+  <si>
+    <t>Westkante:
+![Situationsplan Westkante](https://www.stadt-zuerich.ch/content/dam/web/de/politik-verwaltung/statistik-und-daten/open-government-data/bilder_nwa/datenkatalog/vbz/vbz_Situation_Westkante.PNG)
+Ostkante:
+![Situationsplan/Ostkante](https://www.stadt-zuerich.ch/content/dam/web/de/politik-verwaltung/statistik-und-daten/open-government-data/bilder_nwa/datenkatalog/vbz/vbz_Situation_Ostkante.PNG)</t>
   </si>
 </sst>
 </file>
@@ -1949,8 +1949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2307,7 +2307,7 @@
         <v>51</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C21" s="39" t="s">
         <v>187</v>
@@ -2326,7 +2326,7 @@
         <v>210</v>
       </c>
       <c r="C22" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="7"/>
@@ -2340,7 +2340,7 @@
         <v>184</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="7"/>
@@ -2356,7 +2356,7 @@
         <v>183</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D24" s="43"/>
       <c r="E24" s="7"/>
@@ -3232,6 +3232,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008CBAF0EEED2F5B4AB4463B97C2AD2B71" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="d2bc9691d179cb44d4ba77bdf8fcfb4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c4a6dd5ef775a5269b08f7de37f93f">
     <xsd:element name="properties">
@@ -3345,12 +3351,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3361,6 +3361,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3376,21 +3391,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
   <ds:schemaRefs>

</xml_diff>